<commit_message>
I learned how to import the excel to workbook, read and add values
</commit_message>
<xml_diff>
--- a/Investment_dataset.xlsx
+++ b/Investment_dataset.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,16 @@
     <row r="6">
       <c r="A6" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The information received from the bot is added to the file
</commit_message>
<xml_diff>
--- a/Investment_dataset.xlsx
+++ b/Investment_dataset.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,36 @@
     <row r="8">
       <c r="A8" t="n">
         <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>15</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024.05.10</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>